<commit_message>
I have one routine working. Won't scale
</commit_message>
<xml_diff>
--- a/BroadcastFirstColumn.xlsx
+++ b/BroadcastFirstColumn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{919DCE66-4E2A-481E-A641-A9C67AF4AC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1A83C242-7DC5-4F0D-815B-CA21295265E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <definedName name="_fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat, _xlfn.LET(_xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , -1), _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , 1), _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , -1), _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , 1), IF(_xlpm.xmin = _xlpm.xmax, _xlpm.ymin, (_xlpm.ymin * (_xlpm.xmax - _xlpm.x) + _xlpm.ymax * (_xlpm.x - _xlpm.xmin)) / (_xlpm.xmax - _xlpm.xmin))))</definedName>
     <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode, IF(COLUMNS(_xlpm.lookup_value) = 1, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode), _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)), IFERROR(INDEX(_xlpm.return_array, _xlfn.SEQUENCE(ROWS(_xlpm.return_array)), _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found))))</definedName>
     <definedName name="_fUP">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._f, _xlfn.LAMBDA(_xlpm.z, INDEX(_xlpm.z, _xlfn.SEQUENCE(ROWS(_xlpm.z), 1, ROWS(_xlpm.z), -1))), _xlpm._arr, _xlpm._f(_xlpm.arr), _xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlpm._f(_xlfn.SCAN(_xlpm._ini, _xlpm._arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v))))))</definedName>
+    <definedName name="_nAlt">Report!$H$7:$M$9</definedName>
     <definedName name="_nData">Report!$B$7:$E$10</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
@@ -941,10 +942,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A5:M49"/>
+  <dimension ref="A5:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -1166,119 +1167,182 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B32)</f>
+        <v>=MAP(_nData,LAMBDA(x,x&amp;@+x:B32))</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="str" cm="1">
-        <f t="array" ref="B32:D35">_xlfn.DROP(_xlfn.MAP(_nData,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:B32))),,1)</f>
+        <f t="array" ref="B32:E35">_xlfn.MAP(_nData,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:B32)))</f>
+        <v>AA</v>
+      </c>
+      <c r="C32" t="str">
         <v>1A</v>
       </c>
-      <c r="C32" t="str">
+      <c r="D32" t="str">
         <v>2A</v>
       </c>
-      <c r="D32" t="str">
+      <c r="E32" t="str">
         <v>3A</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
+        <v>BB</v>
+      </c>
+      <c r="C33" t="str">
         <v>4B</v>
       </c>
-      <c r="C33" t="str">
+      <c r="D33" t="str">
         <v>5B</v>
       </c>
-      <c r="D33" t="str">
+      <c r="E33" t="str">
         <v>6B</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
+        <v>CC</v>
+      </c>
+      <c r="C34" t="str">
         <v>7C</v>
       </c>
-      <c r="C34" t="str">
+      <c r="D34" t="str">
         <v>8C</v>
       </c>
-      <c r="D34" t="str">
+      <c r="E34" t="str">
         <v>9C</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
+        <v>DD</v>
+      </c>
+      <c r="C35" t="str">
         <v>10D</v>
       </c>
-      <c r="C35" t="str">
+      <c r="D35" t="str">
         <v>11D</v>
       </c>
-      <c r="D35" t="str">
+      <c r="E35" t="str">
         <v>12D</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="str" cm="1">
-        <f t="array" ref="B38:B49">_xlfn.TOCOL(_xlfn.ANCHORARRAY(B32))</f>
+        <f t="array" ref="B38:D41">_xlfn.DROP(_xlfn.ANCHORARRAY(B32),,1)</f>
         <v>1A</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="str">
+        <v>2A</v>
+      </c>
+      <c r="D38" t="str">
+        <v>3A</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
+        <v>4B</v>
+      </c>
+      <c r="C39" t="str">
+        <v>5B</v>
+      </c>
+      <c r="D39" t="str">
+        <v>6B</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <v>7C</v>
+      </c>
+      <c r="C40" t="str">
+        <v>8C</v>
+      </c>
+      <c r="D40" t="str">
+        <v>9C</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <v>10D</v>
+      </c>
+      <c r="C41" t="str">
+        <v>11D</v>
+      </c>
+      <c r="D41" t="str">
+        <v>12D</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="str" cm="1">
+        <f t="array" ref="B43:B54">_xlfn.TOCOL(_xlfn.ANCHORARRAY(B38))</f>
+        <v>1A</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
         <v>2A</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="str">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
         <v>3A</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="str">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="str">
         <v>4B</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="str">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="str">
         <v>5B</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="str">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
         <v>6B</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="str">
-        <v>7C</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="str">
-        <v>8C</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="str">
-        <v>9C</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="str">
-        <v>10D</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="str">
-        <v>11D</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
+        <v>7C</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="str">
+        <v>8C</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="str">
+        <v>9C</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
+        <v>10D</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="str">
+        <v>11D</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="str">
         <v>12D</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I think I finally understand the implicit intersection
</commit_message>
<xml_diff>
--- a/BroadcastFirstColumn.xlsx
+++ b/BroadcastFirstColumn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1A83C242-7DC5-4F0D-815B-CA21295265E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{BF2BDCB1-1AF8-4A3F-9982-E4C9281BFC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Alternate</t>
+  </si>
+  <si>
+    <t>Key oservation. The result array must be in the same</t>
+  </si>
+  <si>
+    <t>column as the data. This is very limiting.</t>
   </si>
 </sst>
 </file>
@@ -253,10 +262,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comment" xfId="8" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -718,6 +728,109 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Freeform: Shape 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC538E08-E4D2-BA23-4CDE-3B090BECF71F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3206750" y="7556500"/>
+          <a:ext cx="996950" cy="1549400"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 0 w 996950"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 1549400"/>
+            <a:gd name="connsiteX1" fmla="*/ 203200 w 996950"/>
+            <a:gd name="connsiteY1" fmla="*/ 850900 h 1549400"/>
+            <a:gd name="connsiteX2" fmla="*/ 996950 w 996950"/>
+            <a:gd name="connsiteY2" fmla="*/ 1549400 h 1549400"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="996950" h="1549400">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="18521" y="296333"/>
+                <a:pt x="37042" y="592667"/>
+                <a:pt x="203200" y="850900"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="369358" y="1109133"/>
+                <a:pt x="683154" y="1329266"/>
+                <a:pt x="996950" y="1549400"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -942,10 +1055,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A5:M54"/>
+  <dimension ref="A5:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1103,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1111,7 +1224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1248,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -1143,7 +1256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -1151,7 +1264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -1167,23 +1280,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G29" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(B32)</f>
-        <v>=MAP(_nData,LAMBDA(x,x&amp;@+x:B32))</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="str" cm="1">
         <f t="array" ref="B32:E35">_xlfn.MAP(_nData,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:B32)))</f>
         <v>AA</v>
@@ -1197,8 +1304,21 @@
       <c r="E32" t="str">
         <v>3A</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="str" cm="1">
+        <f t="array" ref="G32:J35">_xlfn.MAP(_nData,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:G32)))</f>
+        <v>AA</v>
+      </c>
+      <c r="H32" t="str">
+        <v>11</v>
+      </c>
+      <c r="I32" t="str">
+        <v>22</v>
+      </c>
+      <c r="J32" t="str">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <v>BB</v>
       </c>
@@ -1211,8 +1331,20 @@
       <c r="E33" t="str">
         <v>6B</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <v>BB</v>
+      </c>
+      <c r="H33" t="str">
+        <v>44</v>
+      </c>
+      <c r="I33" t="str">
+        <v>55</v>
+      </c>
+      <c r="J33" t="str">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <v>CC</v>
       </c>
@@ -1225,8 +1357,20 @@
       <c r="E34" t="str">
         <v>9C</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <v>CC</v>
+      </c>
+      <c r="H34" t="str">
+        <v>77</v>
+      </c>
+      <c r="I34" t="str">
+        <v>88</v>
+      </c>
+      <c r="J34" t="str">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <v>DD</v>
       </c>
@@ -1239,8 +1383,20 @@
       <c r="E35" t="str">
         <v>12D</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <v>DD</v>
+      </c>
+      <c r="H35" t="str">
+        <v>1010</v>
+      </c>
+      <c r="I35" t="str">
+        <v>1111</v>
+      </c>
+      <c r="J35" t="str">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="str" cm="1">
         <f t="array" ref="B38:D41">_xlfn.DROP(_xlfn.ANCHORARRAY(B32),,1)</f>
         <v>1A</v>
@@ -1251,8 +1407,12 @@
       <c r="D38" t="str">
         <v>3A</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B32)</f>
+        <v>=MAP(_nData,LAMBDA(x,x&amp;@+x:B32))</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <v>4B</v>
       </c>
@@ -1262,8 +1422,12 @@
       <c r="D39" t="str">
         <v>6B</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H56)</f>
+        <v>=MAP(H7:K9,LAMBDA(x,x&amp;@+x:H56))</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <v>7C</v>
       </c>
@@ -1274,7 +1438,7 @@
         <v>9C</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <v>10D</v>
       </c>
@@ -1285,65 +1449,170 @@
         <v>12D</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" t="str" cm="1">
         <f t="array" ref="B43:B54">_xlfn.TOCOL(_xlfn.ANCHORARRAY(B38))</f>
         <v>1A</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <v>2A</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <v>3A</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <v>4B</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <v>5B</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <v>6B</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <v>7C</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <v>8C</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <v>9C</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <v>10D</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <v>11D</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <v>12D</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" t="str" cm="1">
+        <f t="array" ref="B56:E59">_xlfn.MAP(_nData,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:B56)))</f>
+        <v>AA</v>
+      </c>
+      <c r="C56" t="str">
+        <v>1A</v>
+      </c>
+      <c r="D56" t="str">
+        <v>2A</v>
+      </c>
+      <c r="E56" t="str">
+        <v>3A</v>
+      </c>
+      <c r="H56" t="str" cm="1">
+        <f t="array" ref="H56:K58">_xlfn.MAP(H7:K9,_xlfn.LAMBDA(_xlpm.x,_xlpm.x&amp;_xlfn.SINGLE(+_xlpm.x:H56)))</f>
+        <v>EE</v>
+      </c>
+      <c r="I56" t="str">
+        <v>1E</v>
+      </c>
+      <c r="J56" t="str">
+        <v>2E</v>
+      </c>
+      <c r="K56" t="str">
+        <v>3E</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
+        <v>BB</v>
+      </c>
+      <c r="C57" t="str">
+        <v>4B</v>
+      </c>
+      <c r="D57" t="str">
+        <v>5B</v>
+      </c>
+      <c r="E57" t="str">
+        <v>6B</v>
+      </c>
+      <c r="H57" t="str">
+        <v>FF</v>
+      </c>
+      <c r="I57" t="str">
+        <v>6F</v>
+      </c>
+      <c r="J57" t="str">
+        <v>7F</v>
+      </c>
+      <c r="K57" t="str">
+        <v>8F</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" t="str">
+        <v>CC</v>
+      </c>
+      <c r="C58" t="str">
+        <v>7C</v>
+      </c>
+      <c r="D58" t="str">
+        <v>8C</v>
+      </c>
+      <c r="E58" t="str">
+        <v>9C</v>
+      </c>
+      <c r="H58" t="str">
+        <v>GG</v>
+      </c>
+      <c r="I58" t="str">
+        <v>11G</v>
+      </c>
+      <c r="J58" t="str">
+        <v>12G</v>
+      </c>
+      <c r="K58" t="str">
+        <v>13G</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" t="str">
+        <v>DD</v>
+      </c>
+      <c r="C59" t="str">
+        <v>10D</v>
+      </c>
+      <c r="D59" t="str">
+        <v>11D</v>
+      </c>
+      <c r="E59" t="str">
+        <v>12D</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solution with Expand function
</commit_message>
<xml_diff>
--- a/BroadcastFirstColumn.xlsx
+++ b/BroadcastFirstColumn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{BF2BDCB1-1AF8-4A3F-9982-E4C9281BFC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{64A44873-1E21-46C1-A28F-C58EA61303ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -1055,10 +1055,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A5:M62"/>
+  <dimension ref="A5:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1613,6 +1613,298 @@
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="str" cm="1">
+        <f t="array" ref="B69:B80">_xlfn.LET(_xlpm._c,COLUMNS(_nData)-1,_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TAKE(_nData,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.EXPAND(_xlpm.v,_xlpm._c,1,_xlpm.v)))),1))</f>
+        <v>A</v>
+      </c>
+      <c r="C69" cm="1">
+        <f t="array" ref="C69:C80">_xlfn.TOCOL(_xlfn.DROP(_nData,,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F69" t="str" cm="1">
+        <f t="array" ref="F69:G80">_xlfn.LAMBDA(_xlpm._nData,_xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d,_xlfn.LET(_xlpm._c,COLUMNS(_xlpm._d)-1,_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TAKE(_xlpm._d,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.EXPAND(_xlpm.v,_xlpm._c,1,_xlpm.v)))),1))),
+     _xlfn.HSTACK(_xlpm.f(_xlpm._nData),_xlfn.TOCOL(_xlfn.DROP(_xlpm._nData,,1)))
+))(_nData)</f>
+        <v>A</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="I69" t="str" cm="1">
+        <f t="array" ref="I69:J83">_xlfn.LAMBDA(_xlpm._nData,_xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d,_xlfn.LET(_xlpm._c,COLUMNS(_xlpm._d)-1,_xlfn.DROP(_xlfn.REDUCE("",_xlfn.TAKE(_xlpm._d,,1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.EXPAND(_xlpm.v,_xlpm._c,1,_xlpm.v)))),1))),
+     _xlfn.HSTACK(_xlpm.f(_xlpm._nData),_xlfn.TOCOL(_xlfn.DROP(_xlpm._nData,,1)))
+))(_nAlt)</f>
+        <v>E</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="str">
+        <v>A</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="str">
+        <v>A</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="I70" t="str">
+        <v>E</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="str">
+        <v>A</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="F71" t="str">
+        <v>A</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="I71" t="str">
+        <v>E</v>
+      </c>
+      <c r="J71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="str">
+        <v>B</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="F72" t="str">
+        <v>B</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="I72" t="str">
+        <v>E</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="str">
+        <v>B</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+      <c r="F73" t="str">
+        <v>B</v>
+      </c>
+      <c r="G73">
+        <v>5</v>
+      </c>
+      <c r="I73" t="str">
+        <v>E</v>
+      </c>
+      <c r="J73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" t="str">
+        <v>B</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="F74" t="str">
+        <v>B</v>
+      </c>
+      <c r="G74">
+        <v>6</v>
+      </c>
+      <c r="I74" t="str">
+        <v>F</v>
+      </c>
+      <c r="J74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" t="str">
+        <v>C</v>
+      </c>
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="F75" t="str">
+        <v>C</v>
+      </c>
+      <c r="G75">
+        <v>7</v>
+      </c>
+      <c r="I75" t="str">
+        <v>F</v>
+      </c>
+      <c r="J75">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" t="str">
+        <v>C</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+      <c r="F76" t="str">
+        <v>C</v>
+      </c>
+      <c r="G76">
+        <v>8</v>
+      </c>
+      <c r="I76" t="str">
+        <v>F</v>
+      </c>
+      <c r="J76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="str">
+        <v>C</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="F77" t="str">
+        <v>C</v>
+      </c>
+      <c r="G77">
+        <v>9</v>
+      </c>
+      <c r="I77" t="str">
+        <v>F</v>
+      </c>
+      <c r="J77">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" t="str">
+        <v>D</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="F78" t="str">
+        <v>D</v>
+      </c>
+      <c r="G78">
+        <v>10</v>
+      </c>
+      <c r="I78" t="str">
+        <v>F</v>
+      </c>
+      <c r="J78">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" t="str">
+        <v>D</v>
+      </c>
+      <c r="C79">
+        <v>11</v>
+      </c>
+      <c r="F79" t="str">
+        <v>D</v>
+      </c>
+      <c r="G79">
+        <v>11</v>
+      </c>
+      <c r="I79" t="str">
+        <v>G</v>
+      </c>
+      <c r="J79">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" t="str">
+        <v>D</v>
+      </c>
+      <c r="C80">
+        <v>12</v>
+      </c>
+      <c r="F80" t="str">
+        <v>D</v>
+      </c>
+      <c r="G80">
+        <v>12</v>
+      </c>
+      <c r="I80" t="str">
+        <v>G</v>
+      </c>
+      <c r="J80">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I81" t="str">
+        <v>G</v>
+      </c>
+      <c r="J81">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I82" t="str">
+        <v>G</v>
+      </c>
+      <c r="J82">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I83" t="str">
+        <v>G</v>
+      </c>
+      <c r="J83">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is my function
</commit_message>
<xml_diff>
--- a/BroadcastFirstColumn.xlsx
+++ b/BroadcastFirstColumn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{64A44873-1E21-46C1-A28F-C58EA61303ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{6853495A-3BCB-4A93-B2A2-E55B7CF41345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -1058,7 +1058,7 @@
   <dimension ref="A5:M83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>